<commit_message>
vault backup: 2024-11-12 12:45:03
</commit_message>
<xml_diff>
--- a/2024-2/Evaluación de proyectos/Excels/Estudio_C4.xlsx
+++ b/2024-2/Evaluación de proyectos/Excels/Estudio_C4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IVAN\Desktop\Codes\Apuntes_2024\2024-2\Evaluación de proyectos\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivaaan\Desktop\git\Apuntes_2024\2024-2\Evaluación de proyectos\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131AA0D4-A83E-40F9-93D6-B8FC5BF67CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9DC0B7-843E-4C65-96E4-AEDA055616F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{53A1CBE7-EF24-4647-958C-2AED564643CD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{53A1CBE7-EF24-4647-958C-2AED564643CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Materia" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
   <si>
     <t>B/C</t>
   </si>
@@ -191,15 +191,6 @@
     <t>VALOR ENERGIA</t>
   </si>
   <si>
-    <t>PERIODO (AÑOS)</t>
-  </si>
-  <si>
-    <t>BENEFICIO</t>
-  </si>
-  <si>
-    <t>MANTENCIÓN</t>
-  </si>
-  <si>
     <t>CONSUMO TOTAL KW/H</t>
   </si>
   <si>
@@ -258,11 +249,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;\-#,##0"/>
+  <numFmts count="3">
     <numFmt numFmtId="42" formatCode="_ &quot;$&quot;* #,##0_ ;_ &quot;$&quot;* \-#,##0_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="172" formatCode="0.000"/>
-    <numFmt numFmtId="176" formatCode="_ &quot;$&quot;* #,##0.00_ ;_ &quot;$&quot;* \-#,##0.00_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="_ &quot;$&quot;* #,##0.00_ ;_ &quot;$&quot;* \-#,##0.00_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -388,12 +378,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -408,78 +395,66 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -915,12 +890,12 @@
   <dimension ref="G4:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G4" t="s">
         <v>0</v>
       </c>
@@ -928,7 +903,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="7:8" x14ac:dyDescent="0.3">
       <c r="H5" t="s">
         <v>26</v>
       </c>
@@ -944,171 +919,171 @@
   <dimension ref="G2:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="7:13" x14ac:dyDescent="0.3">
       <c r="G2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="7:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G3" s="1" t="s">
+    <row r="3" spans="7:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="11" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G11" s="4" t="s">
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+    </row>
+    <row r="4" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+    </row>
+    <row r="5" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+    </row>
+    <row r="6" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+    </row>
+    <row r="7" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+    </row>
+    <row r="8" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+    </row>
+    <row r="9" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+    </row>
+    <row r="11" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G11" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="5">
+      <c r="H11" s="18"/>
+      <c r="I11" s="4">
         <v>500000</v>
       </c>
     </row>
-    <row r="12" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G12" s="4" t="s">
+    <row r="12" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G12" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="5">
+      <c r="H12" s="18"/>
+      <c r="I12" s="4">
         <v>200000</v>
       </c>
     </row>
-    <row r="13" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G13" s="8" t="s">
+    <row r="13" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G13" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="9">
+      <c r="H13" s="17"/>
+      <c r="I13" s="6">
         <f>I11-I12</f>
         <v>300000</v>
       </c>
     </row>
-    <row r="14" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G15" s="4" t="s">
+    <row r="14" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G15" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="6">
+      <c r="H15" s="18"/>
+      <c r="I15" s="5">
         <v>0.06</v>
       </c>
     </row>
-    <row r="16" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G16" s="4" t="s">
+    <row r="16" spans="7:13" x14ac:dyDescent="0.3">
+      <c r="G16" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="5">
+      <c r="H16" s="18"/>
+      <c r="I16" s="4">
         <v>1500000</v>
       </c>
     </row>
-    <row r="17" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G17" s="4" t="s">
+    <row r="17" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G17" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="7">
+      <c r="H17" s="18"/>
+      <c r="I17" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G18" s="8" t="s">
+    <row r="18" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G18" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="8"/>
-      <c r="I18" s="9">
+      <c r="H18" s="17"/>
+      <c r="I18" s="6">
         <f>-PMT(I15,I17,I16)</f>
         <v>203801.93733057575</v>
       </c>
     </row>
-    <row r="20" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G20" s="10" t="s">
+    <row r="20" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G20" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="10"/>
-      <c r="I20" s="13">
+      <c r="H20" s="19"/>
+      <c r="I20" s="8">
         <v>50000</v>
       </c>
     </row>
-    <row r="23" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G23" s="12" t="s">
+    <row r="23" spans="7:10" x14ac:dyDescent="0.3">
+      <c r="G23" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="12"/>
-      <c r="I23" s="14">
+      <c r="H23" s="16"/>
+      <c r="I23" s="9">
         <f>I13/(I18+I20)</f>
         <v>1.1820240741868393</v>
       </c>
@@ -1116,13 +1091,16 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="7:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G24" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="G3:M9"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G15:H15"/>
@@ -1130,9 +1108,6 @@
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G3:M9"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1147,139 +1122,139 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="7" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="16" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="18"/>
+      <c r="B7" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5">
+      <c r="C7" s="18"/>
+      <c r="D7" s="4">
         <v>4000000</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>6000000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="25" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="18"/>
+      <c r="B8" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="5">
+      <c r="C8" s="26"/>
+      <c r="D8" s="4">
         <v>1250000</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>1000000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="25" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="18"/>
+      <c r="B9" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="5">
+      <c r="C9" s="26"/>
+      <c r="D9" s="4">
         <v>200000</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>120000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="16" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="18"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="18"/>
+      <c r="B11" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="6">
+      <c r="C11" s="18"/>
+      <c r="D11" s="5">
         <v>0.08</v>
       </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="16" t="s">
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="18"/>
+      <c r="B12" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="7">
+      <c r="C12" s="18"/>
+      <c r="D12" s="3">
         <v>20</v>
       </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="E12" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="21" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="22"/>
-      <c r="D14" s="13">
+      <c r="D14" s="8">
         <f>-PMT(D11,D12,D7)</f>
         <v>407408.83529260248</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="8">
         <f>-PMT(D11,D12,E7)</f>
         <v>611113.25293890375</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="26" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="24"/>
+      <c r="B15" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="22"/>
-      <c r="D15" s="14">
+      <c r="D15" s="9">
         <f>D8/(D14+D9)</f>
         <v>2.0579219915328482</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="13">
         <f>E8/(E14+E9)</f>
         <v>1.3677771480413392</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="24"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="25"/>
       <c r="B17" t="s">
         <v>25</v>
       </c>
@@ -1304,18 +1279,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043BD017-AE0D-4238-8516-9D619A871FDA}">
   <dimension ref="B4:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22:J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="30" t="s">
         <v>30</v>
       </c>
@@ -1329,7 +1304,7 @@
       <c r="J4" s="30"/>
       <c r="K4" s="30"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="30"/>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -1341,7 +1316,7 @@
       <c r="J5" s="30"/>
       <c r="K5" s="30"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -1353,7 +1328,7 @@
       <c r="J6" s="30"/>
       <c r="K6" s="30"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="30"/>
       <c r="C7" s="30"/>
       <c r="D7" s="30"/>
@@ -1365,7 +1340,7 @@
       <c r="J7" s="30"/>
       <c r="K7" s="30"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
@@ -1377,7 +1352,7 @@
       <c r="J8" s="30"/>
       <c r="K8" s="30"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="30"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -1389,7 +1364,7 @@
       <c r="J9" s="30"/>
       <c r="K9" s="30"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="30"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
@@ -1401,7 +1376,7 @@
       <c r="J10" s="30"/>
       <c r="K10" s="30"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="30"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
@@ -1413,7 +1388,7 @@
       <c r="J11" s="30"/>
       <c r="K11" s="30"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="30"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
@@ -1425,288 +1400,208 @@
       <c r="J12" s="30"/>
       <c r="K12" s="30"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="8" t="s">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C14" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="H14" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C15" s="4" t="s">
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="H14" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C15" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="7">
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="3">
         <v>87.8</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="H15" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="I15" s="21"/>
-      <c r="J15" s="20">
+      <c r="I15" s="29"/>
+      <c r="J15" s="11">
         <f>ROUNDDOWN(F15*1000/F16,0)</f>
         <v>1310</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C16" s="4" t="s">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C16" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="7">
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="3">
         <v>67</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="20">
+      <c r="I16" s="29"/>
+      <c r="J16" s="11">
         <f>J15*2</f>
         <v>2620</v>
       </c>
     </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C17" s="4" t="s">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C17" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="5">
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="4">
         <v>3500</v>
       </c>
-      <c r="H17" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" s="21"/>
-      <c r="J17" s="20">
+      <c r="H17" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="29"/>
+      <c r="J17" s="11">
         <f>J16*F20</f>
         <v>1048</v>
       </c>
     </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C18" s="4" t="s">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C18" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="7">
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="3">
         <v>2</v>
       </c>
-      <c r="H18" s="21" t="s">
+      <c r="H18" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="I18" s="21"/>
-      <c r="J18" s="20">
+      <c r="I18" s="29"/>
+      <c r="J18" s="11">
         <f>F21*F22</f>
         <v>4380</v>
       </c>
     </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C19" s="4" t="s">
+    <row r="19" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C19" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="7">
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="3">
         <v>400</v>
       </c>
-      <c r="H19" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="I19" s="21"/>
-      <c r="J19" s="20">
+      <c r="H19" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" s="29"/>
+      <c r="J19" s="11">
         <f>J18*J17</f>
         <v>4590240</v>
       </c>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="7">
+    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C20" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="3">
         <f>F19/1000</f>
         <v>0.4</v>
       </c>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="I20" s="21"/>
-      <c r="J20" s="31">
+      <c r="I20" s="29"/>
+      <c r="J20" s="14">
         <f>J19*0.08</f>
         <v>367219.20000000001</v>
       </c>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C21" s="15" t="s">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C21" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="7">
+      <c r="D21" s="27"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="3">
         <v>12</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="15" t="s">
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C22" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="7">
+      <c r="D22" s="27"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="3">
         <v>365</v>
       </c>
-      <c r="H22" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="I22" s="21"/>
-      <c r="J22" s="31">
-        <f>F17*J15</f>
-        <v>4585000</v>
-      </c>
-    </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C23" s="15" t="s">
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C23" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="33">
+      <c r="D23" s="27"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="15">
         <v>0.08</v>
       </c>
-      <c r="H23" s="21" t="s">
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C24" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="27"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C25" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="27"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="4">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C26" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="I23" s="21"/>
-      <c r="J23" s="32">
-        <f>F26</f>
+      <c r="D26" s="27"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="5">
         <v>0.06</v>
       </c>
     </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="7">
-        <v>247</v>
-      </c>
-      <c r="H24" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="I24" s="21"/>
-      <c r="J24" s="20">
-        <f>F27</f>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C27" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="27"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="5">
-        <v>4500</v>
-      </c>
-      <c r="H25" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="I25" s="34"/>
-      <c r="J25" s="35">
-        <f>-PMT(J23,J24,J22)</f>
-        <v>1088462.4959770043</v>
-      </c>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="6">
-        <v>0.06</v>
-      </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C27" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="7">
-        <v>5</v>
-      </c>
-      <c r="H27" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="I27" s="21"/>
-      <c r="J27" s="31">
-        <f>F25*F24</f>
-        <v>1111500</v>
-      </c>
-    </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="H28" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="21"/>
-      <c r="J28" s="31">
-        <f>J20</f>
-        <v>367219.20000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="H29" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="I29" s="34"/>
-      <c r="J29" s="36">
-        <f>J27/(J25+J28)</f>
-        <v>0.76355978307056949</v>
-      </c>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.3">
       <c r="K29" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="C22:E22"/>
+  <mergeCells count="22">
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C19:E19"/>
@@ -1717,6 +1612,18 @@
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1726,136 +1633,136 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E79024-F2FA-4725-8CC7-96DE84AC29D6}">
   <dimension ref="B2:V14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-    </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="R3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="S3" s="11">
+        <v>53</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="R3" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="S3" s="7">
         <v>1</v>
       </c>
-      <c r="T3" s="11">
+      <c r="T3" s="7">
         <v>2</v>
       </c>
-      <c r="U3" s="11">
+      <c r="U3" s="7">
         <v>3</v>
       </c>
-      <c r="V3" s="11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C4" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="V3" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="C4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="R4" s="4"/>
-      <c r="S4" s="11">
+      <c r="R4" s="18"/>
+      <c r="S4" s="7">
         <v>-200</v>
       </c>
-      <c r="T4" s="11">
+      <c r="T4" s="7">
         <v>200</v>
       </c>
-      <c r="U4" s="11">
+      <c r="U4" s="7">
         <v>100</v>
       </c>
-      <c r="V4" s="19">
+      <c r="V4" s="10">
         <f>IRR(S4:U4)</f>
         <v>0.36602540378443837</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C5" s="7" t="s">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="C5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="4">
+        <v>50000</v>
+      </c>
+      <c r="E5" s="4">
+        <v>85000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="C6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.35</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="C10" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="5">
-        <v>50000</v>
-      </c>
-      <c r="E5" s="5">
-        <v>85000</v>
-      </c>
-    </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C6" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0.35</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0.28999999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C10" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="11">
+      <c r="D10" s="31"/>
+      <c r="E10" s="7">
         <v>0.16</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C11" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="13">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="C11" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="31"/>
+      <c r="E11" s="8">
         <v>90000</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C13" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" s="23">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="C13" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="12">
         <f>(D5*D6+(E11-D5)*E10)/E11</f>
         <v>0.26555555555555554</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="23">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="12">
         <f>(E5*E6+(E11-E5)*E10)/E11</f>
         <v>0.28277777777777779</v>
       </c>
       <c r="G14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>